<commit_message>
po nowej istalacji i update 2022-11-08
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/akrg.xlsx
+++ b/Statystyki_2018/Template/akrg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t xml:space="preserve">Ruch spraw</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Ga</t>
   </si>
   <si>
+    <t xml:space="preserve">Ga-KRZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gz</t>
   </si>
   <si>
@@ -54,7 +57,13 @@
     <t xml:space="preserve">Gz p-II</t>
   </si>
   <si>
+    <t xml:space="preserve">Gz-KRZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">WSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSNc</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
@@ -136,24 +145,18 @@
     <t xml:space="preserve">Nieobecności (ilość dni)</t>
   </si>
   <si>
+    <t xml:space="preserve">Sąd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wydział</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miesiąc</t>
+  </si>
+  <si>
     <t xml:space="preserve">ETAT</t>
   </si>
   <si>
-    <t xml:space="preserve">GC merytoryczne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ga merytoryczne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilość sporządzonych uzasadnień</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilość uzasadnień zwróconych po terminie ustawowym bądź przedłużonym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uzasadnienia wygłoszone </t>
-  </si>
-  <si>
     <t xml:space="preserve">rozprawy</t>
   </si>
   <si>
@@ -172,10 +175,25 @@
     <t xml:space="preserve">w tym nieusprawiedliwione</t>
   </si>
   <si>
-    <t xml:space="preserve">w tym nieuspra-wiedliwione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wyznaczenia</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">Wyznaczenia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">(merytoryczne)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -208,15 +226,6 @@
       <t xml:space="preserve"> -  liczba spraw odroczonych</t>
     </r>
   </si>
-  <si>
-    <t xml:space="preserve">Sąd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wydział</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miesiąc</t>
-  </si>
 </sst>
 </file>
 
@@ -225,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -271,6 +280,14 @@
       <charset val="238"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -285,6 +302,14 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -319,14 +344,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
     <fill>
@@ -336,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -362,25 +387,11 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
       <right style="thin">
         <color rgb="FF808080"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -389,7 +400,7 @@
       </left>
       <right style="thin"/>
       <top/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -430,20 +441,20 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,7 +470,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -475,83 +486,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -570,7 +537,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFF2F2F2"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -587,7 +554,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -635,17 +602,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:M16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="AB:AC B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.35"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -664,6 +632,9 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
@@ -685,24 +656,33 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="40.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -710,20 +690,23 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -736,11 +719,14 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -753,11 +739,14 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -770,11 +759,14 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -787,11 +779,14 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -805,10 +800,13 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -822,10 +820,13 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -838,11 +839,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -855,11 +859,14 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -872,11 +879,14 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -889,11 +899,14 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -906,11 +919,14 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -923,12 +939,15 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
@@ -937,13 +956,16 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -956,315 +978,396 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AE5"/>
+  <dimension ref="A2:AE1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AB:AC"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD2" activeCellId="1" sqref="N5:O16 AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1014" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="14" t="s">
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="14" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="16"/>
+      <c r="W2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="12"/>
       <c r="Y2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="Z2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="17" t="s">
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="19" t="s">
+      <c r="AD2" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="20" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="12" t="s">
+      <c r="P3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3" s="14"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="22" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="22" t="s">
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="19"/>
-    </row>
-    <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AA3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="U4" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="V4" s="14"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="Y4" s="12"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD4" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="25" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="25" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" s="25" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" s="25" t="n">
-        <v>7</v>
-      </c>
-      <c r="H5" s="25" t="n">
-        <v>8</v>
-      </c>
-      <c r="I5" s="25" t="n">
-        <v>9</v>
-      </c>
-      <c r="J5" s="25" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" s="25" t="n">
-        <v>11</v>
-      </c>
-      <c r="L5" s="25" t="n">
-        <v>12</v>
-      </c>
-      <c r="M5" s="26" t="n">
-        <v>13</v>
-      </c>
-      <c r="N5" s="26" t="n">
-        <v>14</v>
-      </c>
-      <c r="O5" s="25" t="n">
-        <v>15</v>
-      </c>
-      <c r="P5" s="25" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="25" t="n">
-        <v>17</v>
-      </c>
-      <c r="R5" s="25" t="n">
-        <v>18</v>
-      </c>
-      <c r="S5" s="25" t="n">
-        <v>19</v>
-      </c>
-      <c r="T5" s="25" t="n">
-        <v>20</v>
-      </c>
-      <c r="U5" s="25" t="n">
-        <v>21</v>
-      </c>
-      <c r="V5" s="25" t="n">
-        <v>22</v>
-      </c>
-      <c r="W5" s="25" t="n">
-        <v>23</v>
-      </c>
-      <c r="X5" s="25" t="n">
-        <v>24</v>
-      </c>
-      <c r="Y5" s="25" t="n">
-        <v>25</v>
-      </c>
-      <c r="Z5" s="27" t="n">
-        <v>26</v>
-      </c>
-      <c r="AA5" s="27" t="n">
-        <v>27</v>
-      </c>
-      <c r="AB5" s="27" t="n">
-        <v>28</v>
-      </c>
-      <c r="AC5" s="27" t="n">
-        <v>29</v>
-      </c>
-      <c r="AD5" s="27" t="n">
-        <v>30</v>
-      </c>
-      <c r="AE5" s="27" t="n">
-        <v>31</v>
-      </c>
-    </row>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="1"/>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:R2"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:U3"/>
+    <mergeCell ref="G2:U2"/>
     <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="W2:X3"/>
     <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AB4"/>
-    <mergeCell ref="AC2:AD3"/>
+    <mergeCell ref="AC2:AC4"/>
+    <mergeCell ref="AD2:AD4"/>
     <mergeCell ref="AE2:AE4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="1" sqref="N5:O16 L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="19"/>
+    </row>
+    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="19"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:S2"/>
+    <mergeCell ref="T2:T4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
@@ -1278,174 +1381,11 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="S3:S4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:T4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="1" sqref="AB:AC R2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.89"/>
-  </cols>
-  <sheetData>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="R2:R4"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>